<commit_message>
Updated map of sites
</commit_message>
<xml_diff>
--- a/Midlands CDCs - Copy.xlsx
+++ b/Midlands CDCs - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/WMAP diagnostics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/WMAP diagnostics/WM_Diagnostics_Travel_Time/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="10_ncr:40000_{42A5E3C6-3A39-49E2-876F-8F7433900A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{397E2A14-CE15-47A4-A2F7-D9128B6D771A}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="10_ncr:40000_{42A5E3C6-3A39-49E2-876F-8F7433900A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{591B74BE-CCD0-4BB7-BD41-F6B99089318E}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="1920" windowWidth="16956" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -228,13 +228,37 @@
   </si>
   <si>
     <t>LE5 4PW</t>
+  </si>
+  <si>
+    <t>MRI</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>Ultrasound</t>
+  </si>
+  <si>
+    <t>X-ray</t>
+  </si>
+  <si>
+    <t>Hereford City CDC</t>
+  </si>
+  <si>
+    <t>Hereford</t>
+  </si>
+  <si>
+    <t>HR1 2ER</t>
+  </si>
+  <si>
+    <t>* NEW On Hereford County Hospital site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,13 +287,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -284,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -292,6 +329,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,22 +648,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I1048576"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.44140625" customWidth="1"/>
+    <col min="1" max="1" width="36.77734375" customWidth="1"/>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1"/>
     <col min="4" max="4" width="13.21875" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -637,8 +680,20 @@
       <c r="E1" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -654,8 +709,20 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -671,25 +738,41 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -705,25 +788,41 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -739,8 +838,20 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -756,8 +867,20 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -773,25 +896,49 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -807,8 +954,20 @@
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -824,8 +983,20 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -841,67 +1012,103 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>24</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>30</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
       <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
         <v>24</v>
@@ -912,13 +1119,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
@@ -929,13 +1136,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -944,9 +1151,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E19">
-    <sortCondition descending="1" ref="E1:E19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I20">
+    <sortCondition descending="1" ref="E1:E20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>